<commit_message>
powerpoint work sql and csv upload
</commit_message>
<xml_diff>
--- a/nationwide.xlsx
+++ b/nationwide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Desktop\Class_Files\du-den-data-pt-08-2020-u-c\strange_brew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE9AD5C-35E3-45EC-9748-CF7A0AD18736}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB7A2ED-C107-4287-BE2B-FB410EB2CD61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1830" yWindow="1170" windowWidth="21600" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,211 +25,211 @@
     <t>Beer Style</t>
   </si>
   <si>
+    <t>American-Style Pale Ale</t>
+  </si>
+  <si>
+    <t>American-Style Lager</t>
+  </si>
+  <si>
+    <t>American-Style Stout</t>
+  </si>
+  <si>
+    <t>American-Style Amber/Red Ale</t>
+  </si>
+  <si>
+    <t>American-Style India Pale Ale</t>
+  </si>
+  <si>
+    <t>Porter</t>
+  </si>
+  <si>
+    <t>American-Style Brown Ale</t>
+  </si>
+  <si>
+    <t>South German-Style Hefeweizen</t>
+  </si>
+  <si>
+    <t>Traditional German-Style Bock</t>
+  </si>
+  <si>
+    <t>Light American Wheat Ale or Lager</t>
+  </si>
+  <si>
+    <t>German-Style Oktoberfest</t>
+  </si>
+  <si>
+    <t>Imperial or Double India Pale Ale</t>
+  </si>
+  <si>
+    <t>Other Belgian-Style Ales</t>
+  </si>
+  <si>
+    <t>American-Style Imperial Stout</t>
+  </si>
+  <si>
+    <t>Old Ale</t>
+  </si>
+  <si>
+    <t>German-Style Pilsener</t>
+  </si>
+  <si>
+    <t>Scotch Ale</t>
+  </si>
+  <si>
+    <t>Belgian-Style White</t>
+  </si>
+  <si>
+    <t>Fruit Beer</t>
+  </si>
+  <si>
+    <t>Belgian-Style Fruit Lambic</t>
+  </si>
+  <si>
+    <t>American-Style Light Lager</t>
+  </si>
+  <si>
+    <t>German-Style Schwarzbier</t>
+  </si>
+  <si>
+    <t>Belgian-Style Tripel</t>
+  </si>
+  <si>
+    <t>Golden or Blonde Ale</t>
+  </si>
+  <si>
+    <t>American-Style Barley Wine Ale</t>
+  </si>
+  <si>
+    <t>Extra Special Bitter</t>
+  </si>
+  <si>
+    <t>English-Style Pale Mild Ale</t>
+  </si>
+  <si>
+    <t>Oatmeal Stout</t>
+  </si>
+  <si>
+    <t>French &amp; Belgian-Style Saison</t>
+  </si>
+  <si>
+    <t>German-Style Heller Bock/Maibock</t>
+  </si>
+  <si>
+    <t>Winter Warmer</t>
+  </si>
+  <si>
+    <t>Irish-Style Red Ale</t>
+  </si>
+  <si>
+    <t>Dark American-Belgo-Style Ale</t>
+  </si>
+  <si>
+    <t>German-Style Doppelbock</t>
+  </si>
+  <si>
+    <t>Classic English-Style Pale Ale</t>
+  </si>
+  <si>
+    <t>South German-Style Weizenbock</t>
+  </si>
+  <si>
+    <t>Belgian-Style Dubbel</t>
+  </si>
+  <si>
+    <t>Pumpkin Beer</t>
+  </si>
+  <si>
+    <t>German-Style Brown Ale/Altbier</t>
+  </si>
+  <si>
+    <t>Ordinary Bitter</t>
+  </si>
+  <si>
+    <t>Belgian-Style Pale Strong Ale</t>
+  </si>
+  <si>
+    <t>Sweet Stout</t>
+  </si>
+  <si>
+    <t>American-Style Strong Pale Ale</t>
+  </si>
+  <si>
+    <t>Belgian-Style Dark Strong Ale</t>
+  </si>
+  <si>
+    <t>American-Style Cream Ale or Lager</t>
+  </si>
+  <si>
+    <t>Special Bitter or Best Bitter</t>
+  </si>
+  <si>
+    <t>English-Style India Pale Ale</t>
+  </si>
+  <si>
+    <t>American Rye Ale or Lager</t>
+  </si>
+  <si>
+    <t>Herb and Spice Beer</t>
+  </si>
+  <si>
+    <t>Belgian-Style Quadrupel</t>
+  </si>
+  <si>
+    <t>Belgian-Style Pale Ale</t>
+  </si>
+  <si>
+    <t>Baltic-Style Porter</t>
+  </si>
+  <si>
+    <t>Scottish-Style Light Ale</t>
+  </si>
+  <si>
+    <t>Out of Category</t>
+  </si>
+  <si>
+    <t>Vienna-Style Lager</t>
+  </si>
+  <si>
+    <t>Strong Ale</t>
+  </si>
+  <si>
+    <t>English-Style Dark Mild Ale</t>
+  </si>
+  <si>
+    <t>European Low-Alcohol Lager</t>
+  </si>
+  <si>
+    <t>Bamberg-Style Bock Rauchbier</t>
+  </si>
+  <si>
+    <t>Smoke Beer</t>
+  </si>
+  <si>
+    <t>Classic Irish-Style Dry Stout</t>
+  </si>
+  <si>
+    <t>Foreign (Export)-Style Stout</t>
+  </si>
+  <si>
+    <t>American-Style India Black Ale</t>
+  </si>
+  <si>
+    <t>Specialty Beer</t>
+  </si>
+  <si>
+    <t>American-Style Dark Lager</t>
+  </si>
+  <si>
+    <t>Specialty Honey Lager or Ale</t>
+  </si>
+  <si>
+    <t>Kellerbier - Ale</t>
+  </si>
+  <si>
+    <t>Imperial or Double Red Ale</t>
+  </si>
+  <si>
     <t>Count</t>
-  </si>
-  <si>
-    <t>American-Style Pale Ale</t>
-  </si>
-  <si>
-    <t>American-Style Lager</t>
-  </si>
-  <si>
-    <t>American-Style Stout</t>
-  </si>
-  <si>
-    <t>American-Style Amber/Red Ale</t>
-  </si>
-  <si>
-    <t>American-Style India Pale Ale</t>
-  </si>
-  <si>
-    <t>Porter</t>
-  </si>
-  <si>
-    <t>American-Style Brown Ale</t>
-  </si>
-  <si>
-    <t>South German-Style Hefeweizen</t>
-  </si>
-  <si>
-    <t>Traditional German-Style Bock</t>
-  </si>
-  <si>
-    <t>Light American Wheat Ale or Lager</t>
-  </si>
-  <si>
-    <t>German-Style Oktoberfest</t>
-  </si>
-  <si>
-    <t>Imperial or Double India Pale Ale</t>
-  </si>
-  <si>
-    <t>Other Belgian-Style Ales</t>
-  </si>
-  <si>
-    <t>American-Style Imperial Stout</t>
-  </si>
-  <si>
-    <t>Old Ale</t>
-  </si>
-  <si>
-    <t>German-Style Pilsener</t>
-  </si>
-  <si>
-    <t>Scotch Ale</t>
-  </si>
-  <si>
-    <t>Belgian-Style White</t>
-  </si>
-  <si>
-    <t>Fruit Beer</t>
-  </si>
-  <si>
-    <t>Belgian-Style Fruit Lambic</t>
-  </si>
-  <si>
-    <t>American-Style Light Lager</t>
-  </si>
-  <si>
-    <t>German-Style Schwarzbier</t>
-  </si>
-  <si>
-    <t>Belgian-Style Tripel</t>
-  </si>
-  <si>
-    <t>Golden or Blonde Ale</t>
-  </si>
-  <si>
-    <t>American-Style Barley Wine Ale</t>
-  </si>
-  <si>
-    <t>Extra Special Bitter</t>
-  </si>
-  <si>
-    <t>English-Style Pale Mild Ale</t>
-  </si>
-  <si>
-    <t>Oatmeal Stout</t>
-  </si>
-  <si>
-    <t>French &amp; Belgian-Style Saison</t>
-  </si>
-  <si>
-    <t>German-Style Heller Bock/Maibock</t>
-  </si>
-  <si>
-    <t>Winter Warmer</t>
-  </si>
-  <si>
-    <t>Irish-Style Red Ale</t>
-  </si>
-  <si>
-    <t>Dark American-Belgo-Style Ale</t>
-  </si>
-  <si>
-    <t>German-Style Doppelbock</t>
-  </si>
-  <si>
-    <t>Classic English-Style Pale Ale</t>
-  </si>
-  <si>
-    <t>South German-Style Weizenbock</t>
-  </si>
-  <si>
-    <t>Belgian-Style Dubbel</t>
-  </si>
-  <si>
-    <t>Pumpkin Beer</t>
-  </si>
-  <si>
-    <t>German-Style Brown Ale/Altbier</t>
-  </si>
-  <si>
-    <t>Ordinary Bitter</t>
-  </si>
-  <si>
-    <t>Belgian-Style Pale Strong Ale</t>
-  </si>
-  <si>
-    <t>Sweet Stout</t>
-  </si>
-  <si>
-    <t>American-Style Strong Pale Ale</t>
-  </si>
-  <si>
-    <t>Belgian-Style Dark Strong Ale</t>
-  </si>
-  <si>
-    <t>American-Style Cream Ale or Lager</t>
-  </si>
-  <si>
-    <t>Special Bitter or Best Bitter</t>
-  </si>
-  <si>
-    <t>English-Style India Pale Ale</t>
-  </si>
-  <si>
-    <t>American Rye Ale or Lager</t>
-  </si>
-  <si>
-    <t>Herb and Spice Beer</t>
-  </si>
-  <si>
-    <t>Belgian-Style Quadrupel</t>
-  </si>
-  <si>
-    <t>Belgian-Style Pale Ale</t>
-  </si>
-  <si>
-    <t>Baltic-Style Porter</t>
-  </si>
-  <si>
-    <t>Scottish-Style Light Ale</t>
-  </si>
-  <si>
-    <t>Out of Category</t>
-  </si>
-  <si>
-    <t>Vienna-Style Lager</t>
-  </si>
-  <si>
-    <t>Strong Ale</t>
-  </si>
-  <si>
-    <t>English-Style Dark Mild Ale</t>
-  </si>
-  <si>
-    <t>European Low-Alcohol Lager</t>
-  </si>
-  <si>
-    <t>Bamberg-Style Bock Rauchbier</t>
-  </si>
-  <si>
-    <t>Smoke Beer</t>
-  </si>
-  <si>
-    <t>Classic Irish-Style Dry Stout</t>
-  </si>
-  <si>
-    <t>Foreign (Export)-Style Stout</t>
-  </si>
-  <si>
-    <t>American-Style India Black Ale</t>
-  </si>
-  <si>
-    <t>Specialty Beer</t>
-  </si>
-  <si>
-    <t>American-Style Dark Lager</t>
-  </si>
-  <si>
-    <t>Specialty Honey Lager or Ale</t>
-  </si>
-  <si>
-    <t>Kellerbier - Ale</t>
-  </si>
-  <si>
-    <t>Imperial or Double Red Ale</t>
   </si>
 </sst>
 </file>
@@ -595,26 +595,22 @@
   <dimension ref="A1:B69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>527</v>
@@ -622,7 +618,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>517</v>
@@ -630,7 +626,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>334</v>
@@ -638,7 +634,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>305</v>
@@ -646,7 +642,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>300</v>
@@ -654,7 +650,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>267</v>
@@ -662,7 +658,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>248</v>
@@ -670,7 +666,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>185</v>
@@ -678,7 +674,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>161</v>
@@ -686,7 +682,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>133</v>
@@ -694,7 +690,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>114</v>
@@ -702,7 +698,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>101</v>
@@ -710,7 +706,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>79</v>
@@ -718,7 +714,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>77</v>
@@ -726,7 +722,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>73</v>
@@ -734,7 +730,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>72</v>
@@ -742,7 +738,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>66</v>
@@ -750,7 +746,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>57</v>
@@ -758,7 +754,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>56</v>
@@ -766,7 +762,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>55</v>
@@ -774,7 +770,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>54</v>
@@ -782,7 +778,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>48</v>
@@ -790,7 +786,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>44</v>
@@ -798,7 +794,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>42</v>
@@ -806,7 +802,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>40</v>
@@ -814,7 +810,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27">
         <v>36</v>
@@ -822,7 +818,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28">
         <v>34</v>
@@ -830,7 +826,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>32</v>
@@ -838,7 +834,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30">
         <v>26</v>
@@ -846,7 +842,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31">
         <v>24</v>
@@ -854,7 +850,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32">
         <v>23</v>
@@ -862,7 +858,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33">
         <v>23</v>
@@ -870,7 +866,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34">
         <v>22</v>
@@ -878,7 +874,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35">
         <v>21</v>
@@ -886,7 +882,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36">
         <v>20</v>
@@ -894,7 +890,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37">
         <v>19</v>
@@ -902,7 +898,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38">
         <v>19</v>
@@ -910,7 +906,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39">
         <v>18</v>
@@ -918,7 +914,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40">
         <v>17</v>
@@ -926,7 +922,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41">
         <v>16</v>
@@ -934,7 +930,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42">
         <v>15</v>
@@ -942,7 +938,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43">
         <v>14</v>
@@ -950,7 +946,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44">
         <v>14</v>
@@ -958,7 +954,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45">
         <v>14</v>
@@ -966,7 +962,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46">
         <v>13</v>
@@ -974,7 +970,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47">
         <v>12</v>
@@ -982,7 +978,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48">
         <v>12</v>
@@ -990,7 +986,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49">
         <v>11</v>
@@ -998,7 +994,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50">
         <v>11</v>
@@ -1006,7 +1002,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51">
         <v>10</v>
@@ -1014,7 +1010,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52">
         <v>9</v>
@@ -1022,7 +1018,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -1030,7 +1026,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54">
         <v>3</v>
@@ -1038,7 +1034,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55">
         <v>3</v>
@@ -1046,7 +1042,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56">
         <v>2</v>
@@ -1054,7 +1050,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -1062,7 +1058,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -1070,7 +1066,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -1078,7 +1074,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -1086,7 +1082,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -1094,7 +1090,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -1102,7 +1098,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -1110,7 +1106,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -1118,7 +1114,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -1126,7 +1122,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -1134,7 +1130,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -1142,7 +1138,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -1150,7 +1146,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B69">
         <v>1</v>

</xml_diff>